<commit_message>
Modelo de dados e Dicionário de dados
</commit_message>
<xml_diff>
--- a/Docs/Dicionário de dados.xlsx
+++ b/Docs/Dicionário de dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pocaz\Desktop\projecto-final\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB636EE-8E0A-4177-BB94-AE5F3F97CFAA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AA4113-5F1F-4AEC-AD1E-403AF4044AA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13425" yWindow="8205" windowWidth="15375" windowHeight="7995" xr2:uid="{E92F487F-D945-4D71-8B77-8D0E69DF42A8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="204">
   <si>
     <t>Entidade:</t>
   </si>
@@ -60,9 +60,6 @@
     <t>id_genero</t>
   </si>
   <si>
-    <t>valor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Número único usado para identificar o género </t>
   </si>
   <si>
@@ -138,36 +135,6 @@
     <t>Nome do distrito</t>
   </si>
   <si>
-    <t>Curso Primeira Opção</t>
-  </si>
-  <si>
-    <t>Entidade que guarda as informações sobre o curso de primeira opção</t>
-  </si>
-  <si>
-    <t>id_curso_1a_opcao</t>
-  </si>
-  <si>
-    <t>Número único usado para identificar o curso de primeira opção</t>
-  </si>
-  <si>
-    <t>Nome do curso de primeira opção</t>
-  </si>
-  <si>
-    <t>Curso Segunda Opção</t>
-  </si>
-  <si>
-    <t>Entidade que guarda as informações sobre o curso de segunda opção</t>
-  </si>
-  <si>
-    <t>id_curso_2a_opcao</t>
-  </si>
-  <si>
-    <t>Número único usado para identificar o curso de segunda opção</t>
-  </si>
-  <si>
-    <t>Nome do curso de segunda opção</t>
-  </si>
-  <si>
     <t>Formulário</t>
   </si>
   <si>
@@ -331,6 +298,351 @@
   </si>
   <si>
     <t>Avaliação / Parecer-final</t>
+  </si>
+  <si>
+    <t>id_candidato</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar o candidato</t>
+  </si>
+  <si>
+    <t>id_curso</t>
+  </si>
+  <si>
+    <t>Chave primária / Chave estrangeira</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar os cursos</t>
+  </si>
+  <si>
+    <t>Curso Opção 1</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações que relacionam o candidato com o curso de primeira opção</t>
+  </si>
+  <si>
+    <t>Curso Opção 2</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações que relacionam o candidato com o curso de segunda opção</t>
+  </si>
+  <si>
+    <t>Valores de 1 a 3</t>
+  </si>
+  <si>
+    <t>Candidato</t>
+  </si>
+  <si>
+    <t>Entidade que guarda os dados do candidato</t>
+  </si>
+  <si>
+    <t>Chave Primária</t>
+  </si>
+  <si>
+    <t>25 dígitos</t>
+  </si>
+  <si>
+    <t>Número de identificação fiscal do candidato</t>
+  </si>
+  <si>
+    <t>9 Dígitos</t>
+  </si>
+  <si>
+    <t>NIF</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Género do candidato</t>
+  </si>
+  <si>
+    <t>10 Dígitos</t>
+  </si>
+  <si>
+    <t>Valores possíveis: Masculino ou Feminino</t>
+  </si>
+  <si>
+    <t>Data_nascimento</t>
+  </si>
+  <si>
+    <t>Data de Nascimento do candidato</t>
+  </si>
+  <si>
+    <t>Inscricao_estado</t>
+  </si>
+  <si>
+    <t>Estado da inscrição do candidato</t>
+  </si>
+  <si>
+    <t>Data_candidatura</t>
+  </si>
+  <si>
+    <t>Data de candidatura do candidato</t>
+  </si>
+  <si>
+    <t>Ano_candidatura</t>
+  </si>
+  <si>
+    <t>Ano de candidatura do candidato</t>
+  </si>
+  <si>
+    <t>4 Dígitos</t>
+  </si>
+  <si>
+    <t>Origem</t>
+  </si>
+  <si>
+    <t>Situacao_desemprego</t>
+  </si>
+  <si>
+    <t>Situação de desemprego do candidato</t>
+  </si>
+  <si>
+    <t>Data_anulacao</t>
+  </si>
+  <si>
+    <t>Habilitacoes_Literarias</t>
+  </si>
+  <si>
+    <t>Habilitações literárias do candidato</t>
+  </si>
+  <si>
+    <t>Chave Estrangeira</t>
+  </si>
+  <si>
+    <t>Escola_proveniencia</t>
+  </si>
+  <si>
+    <t>Escola de proveniência do candidato</t>
+  </si>
+  <si>
+    <t>Contacto_telefonico</t>
+  </si>
+  <si>
+    <t>Contacto telefónico do candidato</t>
+  </si>
+  <si>
+    <t>Distrito a que pertence o candidato</t>
+  </si>
+  <si>
+    <t>Freguesia</t>
+  </si>
+  <si>
+    <t>Freguesia a que pertence o candidato</t>
+  </si>
+  <si>
+    <t>Localidade</t>
+  </si>
+  <si>
+    <t>Localidade a que pertence o candidato</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Email do candidato</t>
+  </si>
+  <si>
+    <t>50 Dígitos</t>
+  </si>
+  <si>
+    <t>Curso_Opcao_1</t>
+  </si>
+  <si>
+    <t>Curso_Opcao_2</t>
+  </si>
+  <si>
+    <t>Curso a que o candidato concorre como primeira opção</t>
+  </si>
+  <si>
+    <t>Curso a que o candidato concorre como segunda opção</t>
+  </si>
+  <si>
+    <t>Turma_rs</t>
+  </si>
+  <si>
+    <t>Turma a que o candidato é alocado no momento da inscrição</t>
+  </si>
+  <si>
+    <t>url_ficha_inscricao</t>
+  </si>
+  <si>
+    <t>Url para o ficheiro da ficha de inscrição do candidato</t>
+  </si>
+  <si>
+    <t>url_cartao_cidadao</t>
+  </si>
+  <si>
+    <t>Url para o ficheiro do cartão de cidadão do candidato</t>
+  </si>
+  <si>
+    <t>url_certificado_habilitacoes</t>
+  </si>
+  <si>
+    <t>Url para o ficheiro do certificado de habilitações do candidato</t>
+  </si>
+  <si>
+    <t>url_curriculo</t>
+  </si>
+  <si>
+    <t>Url para o ficheiro do currículo do candidato</t>
+  </si>
+  <si>
+    <t>url_registo_criminal</t>
+  </si>
+  <si>
+    <t>Url para o ficheiro do registo criminal do candidato</t>
+  </si>
+  <si>
+    <t>url_declaracao_emprego</t>
+  </si>
+  <si>
+    <t>Url para o ficheiro da declaração de situação de desemprego do candidato</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>apto</t>
+  </si>
+  <si>
+    <t>categorização</t>
+  </si>
+  <si>
+    <t>data_assessment</t>
+  </si>
+  <si>
+    <t>Observações relativas ao candidato</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações dos cursos disponibilzados</t>
+  </si>
+  <si>
+    <t>Data de início do curso</t>
+  </si>
+  <si>
+    <t>Nome do curso</t>
+  </si>
+  <si>
+    <t>Prova</t>
+  </si>
+  <si>
+    <t>id_prova</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar a prova (?)</t>
+  </si>
+  <si>
+    <t>Data de realização da prova</t>
+  </si>
+  <si>
+    <t>Resultado da prova</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar o candidato que realiza a prova</t>
+  </si>
+  <si>
+    <t>Inventário Vocacional</t>
+  </si>
+  <si>
+    <t>id_inventario</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar o inventário vocacional</t>
+  </si>
+  <si>
+    <t>Data de realização do inventário vocacional</t>
+  </si>
+  <si>
+    <t>Testes Psicotécnicos</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre os testes psicotécnicos realizados pelo candidato</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre o inventário vocacional realizado pelo candidato</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre a prova realizada pelo candidato</t>
+  </si>
+  <si>
+    <t>id_teste_psicotecnico</t>
+  </si>
+  <si>
+    <t>Data de realização dos testes psicotecnicos</t>
+  </si>
+  <si>
+    <t>Assistente de Formação</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre as assistentes de formação</t>
+  </si>
+  <si>
+    <t>id_assistente_formacao</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar a assistente de formação</t>
+  </si>
+  <si>
+    <t>Nome da assistente de formação</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre a turma a que o candidato é alocado no momento da inscrição</t>
+  </si>
+  <si>
+    <t>id_turma_rs</t>
+  </si>
+  <si>
+    <t>Chave estrangeira</t>
+  </si>
+  <si>
+    <t>id_estado_turma</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar o estado da turma</t>
+  </si>
+  <si>
+    <t>Estado da Turma</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre o estado das turmas</t>
+  </si>
+  <si>
+    <t>Nome do estado da turma</t>
+  </si>
+  <si>
+    <t>Entrevistador</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre o entrevistador</t>
+  </si>
+  <si>
+    <t>id_entrevistador</t>
+  </si>
+  <si>
+    <t>Nome do entrevistador</t>
+  </si>
+  <si>
+    <t>Número único usado para identificar o entrevistador</t>
+  </si>
+  <si>
+    <t>Entrevista_Entrevistador</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre as relações entre a entrevista e o entrevistador</t>
+  </si>
+  <si>
+    <t>Chave primária/Chave estrangeira</t>
+  </si>
+  <si>
+    <t>Entrevista</t>
+  </si>
+  <si>
+    <t>Entidade que guarda as informações sobre a entrevista</t>
+  </si>
+  <si>
+    <t>Data de realização da entrevista</t>
   </si>
 </sst>
 </file>
@@ -362,12 +674,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -462,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -518,44 +836,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,16 +1233,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB70AEAC-8C8E-48A3-B572-692385E33AC1}">
-  <dimension ref="B1:G78"/>
+  <dimension ref="B1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -892,15 +1254,15 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -924,7 +1286,7 @@
       <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -934,31 +1296,31 @@
         <v>8</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="G6" s="13"/>
     </row>
@@ -967,13 +1329,13 @@
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="8"/>
       <c r="G9" s="14"/>
     </row>
@@ -999,41 +1361,41 @@
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>20</v>
-      </c>
       <c r="E12" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="G13" s="13"/>
     </row>
@@ -1042,13 +1404,13 @@
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="8"/>
       <c r="G15" s="14"/>
     </row>
@@ -1074,41 +1436,41 @@
       <c r="F17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>26</v>
-      </c>
       <c r="E18" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="G19" s="13"/>
     </row>
@@ -1118,14 +1480,14 @@
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
@@ -1137,53 +1499,53 @@
     </row>
     <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>26</v>
-      </c>
       <c r="E24" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G25" s="13"/>
     </row>
@@ -1193,14 +1555,14 @@
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
@@ -1224,41 +1586,41 @@
       <c r="F29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="30" t="s">
+      <c r="G29" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>33</v>
-      </c>
       <c r="E30" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="G31" s="13"/>
     </row>
@@ -1268,14 +1630,14 @@
         <v>0</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
+        <v>94</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
@@ -1299,43 +1661,45 @@
       <c r="F35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="21"/>
+      <c r="C36" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="5" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="13"/>
+        <v>93</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="36" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1343,14 +1707,14 @@
         <v>0</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
+        <v>96</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
@@ -1374,58 +1738,67 @@
       <c r="F41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
-      <c r="C42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="5" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="13"/>
-    </row>
-    <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>93</v>
+      </c>
+      <c r="E43" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="34"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+    </row>
     <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
+      <c r="D45" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="33"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
@@ -1449,423 +1822,1857 @@
       <c r="F47" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="30" t="s">
+      <c r="G47" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
-      <c r="C48" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="23"/>
-      <c r="C49" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="G49" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="C50" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G50" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G51" s="28" t="s">
-        <v>56</v>
-      </c>
+      <c r="C48" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G48" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+      <c r="C49" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G49" s="27"/>
+    </row>
+    <row r="50" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="4"/>
+      <c r="C50" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G50" s="36"/>
+    </row>
+    <row r="51" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="34"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
     </row>
     <row r="52" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
-      <c r="C52" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
-      <c r="C53" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
       <c r="G53" s="12"/>
     </row>
     <row r="54" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G54" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G56" s="12"/>
+        <v>36</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="21"/>
+      <c r="C56" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G56" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="3" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G57" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="58" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="3" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G58" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="59" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="3" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G59" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="3" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>61</v>
+        <v>14</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="G60" s="12"/>
     </row>
     <row r="61" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="3" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>15</v>
+        <v>52</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="2:7" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
-      <c r="C63" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E63" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="G63" s="29" t="s">
-        <v>86</v>
-      </c>
+    <row r="63" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+      <c r="C63" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G63" s="12"/>
     </row>
     <row r="64" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64" s="29" t="s">
-        <v>86</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G64" s="12"/>
     </row>
     <row r="65" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65" s="29" t="s">
-        <v>86</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" s="12"/>
     </row>
     <row r="66" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G66" s="12"/>
+    </row>
+    <row r="67" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="3" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>15</v>
+        <v>63</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G67" s="29" t="s">
-        <v>86</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G67" s="12"/>
     </row>
     <row r="68" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>91</v>
+        <v>64</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G68" s="12"/>
     </row>
     <row r="69" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>93</v>
+        <v>66</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="E69" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G69" s="12"/>
+    </row>
+    <row r="70" spans="2:7" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="21"/>
+      <c r="C70" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G70" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+      <c r="C71" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F69" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G69" s="12"/>
-    </row>
-    <row r="70" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="4"/>
-      <c r="C70" s="5" t="s">
+      <c r="G71" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="C72" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="C73" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="C74" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+      <c r="C75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G75" s="12"/>
+    </row>
+    <row r="76" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+      <c r="C76" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G76" s="12"/>
+    </row>
+    <row r="77" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="4"/>
+      <c r="C77" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D70" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="13"/>
-    </row>
-    <row r="71" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C71" s="6"/>
-    </row>
-    <row r="72" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C72" s="6"/>
-    </row>
-    <row r="73" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C73" s="6"/>
-    </row>
-    <row r="74" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C74" s="6"/>
-    </row>
-    <row r="75" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C75" s="6"/>
-    </row>
-    <row r="76" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C76" s="6"/>
-    </row>
-    <row r="77" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C77" s="6"/>
-    </row>
-    <row r="78" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C78" s="6"/>
+      <c r="D79" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="33"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="12"/>
+    </row>
+    <row r="81" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="C81" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="C82" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G82" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B83" s="21"/>
+      <c r="C83" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D83" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="G83" s="25"/>
+    </row>
+    <row r="84" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+      <c r="C84" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G84" s="26"/>
+    </row>
+    <row r="85" spans="2:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="21"/>
+      <c r="C85" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E85" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G85" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D86" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G86" s="26"/>
+    </row>
+    <row r="87" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+      <c r="C87" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="39"/>
+    </row>
+    <row r="88" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+      <c r="C88" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G88" s="12"/>
+    </row>
+    <row r="89" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+      <c r="C89" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D89" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G89" s="12"/>
+    </row>
+    <row r="90" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D90" s="40"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="39"/>
+    </row>
+    <row r="91" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B91" s="2"/>
+      <c r="C91" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="38"/>
+      <c r="G91" s="39"/>
+    </row>
+    <row r="92" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B92" s="2"/>
+      <c r="C92" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D92" s="40"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="39"/>
+    </row>
+    <row r="93" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+      <c r="C93" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D93" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+      <c r="C94" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G94" s="12"/>
+    </row>
+    <row r="95" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B95" s="2"/>
+      <c r="C95" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D95" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G95" s="12"/>
+    </row>
+    <row r="96" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B96" s="2"/>
+      <c r="C96" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G96" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B97" s="21"/>
+      <c r="C97" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D97" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G97" s="27"/>
+    </row>
+    <row r="98" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+      <c r="C98" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D98" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G98" s="27"/>
+    </row>
+    <row r="99" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B99" s="2"/>
+      <c r="C99" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G99" s="27"/>
+    </row>
+    <row r="100" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B100" s="2"/>
+      <c r="C100" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D100" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G100" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B101" s="2"/>
+      <c r="C101" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D101" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B102" s="2"/>
+      <c r="C102" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D102" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G102" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B103" s="2"/>
+      <c r="C103" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D103" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G103" s="12"/>
+    </row>
+    <row r="104" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B104" s="2"/>
+      <c r="C104" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D104" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G104" s="12"/>
+    </row>
+    <row r="105" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B105" s="2"/>
+      <c r="C105" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D105" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G105" s="12"/>
+    </row>
+    <row r="106" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B106" s="2"/>
+      <c r="C106" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D106" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G106" s="12"/>
+    </row>
+    <row r="107" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B107" s="2"/>
+      <c r="C107" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D107" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G107" s="12"/>
+    </row>
+    <row r="108" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B108" s="2"/>
+      <c r="C108" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D108" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G108" s="12"/>
+    </row>
+    <row r="109" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B109" s="2"/>
+      <c r="C109" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D109" s="40"/>
+      <c r="E109" s="38"/>
+      <c r="F109" s="38"/>
+      <c r="G109" s="39"/>
+    </row>
+    <row r="110" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B110" s="2"/>
+      <c r="C110" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D110" s="40"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
+      <c r="G110" s="39"/>
+    </row>
+    <row r="111" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B111" s="2"/>
+      <c r="C111" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D111" s="40"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="39"/>
+    </row>
+    <row r="112" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B112" s="2"/>
+      <c r="C112" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D112" s="40"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="39"/>
+    </row>
+    <row r="113" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="4"/>
+      <c r="C113" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F113" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G113" s="13"/>
+    </row>
+    <row r="114" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="E115" s="32"/>
+      <c r="F115" s="32"/>
+      <c r="G115" s="33"/>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="2"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="12"/>
+    </row>
+    <row r="117" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B117" s="2"/>
+      <c r="C117" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G117" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B118" s="2"/>
+      <c r="C118" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D118" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E118" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G118" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B119" s="2"/>
+      <c r="C119" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D119" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E119" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F119" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G119" s="27"/>
+    </row>
+    <row r="120" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B120" s="2"/>
+      <c r="C120" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D120" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E120" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G120" s="27"/>
+    </row>
+    <row r="121" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="4"/>
+      <c r="C121" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D121" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G121" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D123" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="E123" s="32"/>
+      <c r="F123" s="32"/>
+      <c r="G123" s="33"/>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="2"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="12"/>
+    </row>
+    <row r="125" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B125" s="2"/>
+      <c r="C125" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G125" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B126" s="2"/>
+      <c r="C126" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="E126" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F126" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G126" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B127" s="2"/>
+      <c r="C127" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D127" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E127" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F127" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G127" s="27"/>
+    </row>
+    <row r="128" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B128" s="2"/>
+      <c r="C128" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D128" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="E128" s="41"/>
+      <c r="F128" s="41"/>
+      <c r="G128" s="42"/>
+    </row>
+    <row r="129" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B129" s="4"/>
+      <c r="C129" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D129" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E129" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F129" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G129" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="131" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D131" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="E131" s="32"/>
+      <c r="F131" s="32"/>
+      <c r="G131" s="33"/>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="2"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="17"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="12"/>
+    </row>
+    <row r="133" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B133" s="2"/>
+      <c r="C133" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G133" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B134" s="2"/>
+      <c r="C134" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D134" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="E134" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F134" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G134" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B135" s="2"/>
+      <c r="C135" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D135" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="E135" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F135" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G135" s="27"/>
+    </row>
+    <row r="136" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B136" s="2"/>
+      <c r="C136" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D136" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="E136" s="41"/>
+      <c r="F136" s="41"/>
+      <c r="G136" s="42"/>
+    </row>
+    <row r="137" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="4"/>
+      <c r="C137" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D137" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E137" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G137" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="139" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D139" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="E139" s="32"/>
+      <c r="F139" s="32"/>
+      <c r="G139" s="33"/>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B140" s="2"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="17"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="12"/>
+    </row>
+    <row r="141" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B141" s="2"/>
+      <c r="C141" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G141" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B142" s="2"/>
+      <c r="C142" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D142" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E142" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F142" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G142" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="2"/>
+      <c r="C143" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D143" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E143" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G143" s="27"/>
+    </row>
+    <row r="144" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="44"/>
+      <c r="C144" s="45"/>
+      <c r="D144" s="46"/>
+      <c r="E144" s="47"/>
+      <c r="F144" s="47"/>
+      <c r="G144" s="47"/>
+    </row>
+    <row r="145" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D145" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E145" s="32"/>
+      <c r="F145" s="32"/>
+      <c r="G145" s="33"/>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B146" s="2"/>
+      <c r="C146" s="9"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="12"/>
+    </row>
+    <row r="147" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B147" s="2"/>
+      <c r="C147" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G147" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+      <c r="C148" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D148" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E148" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F148" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G148" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+      <c r="C149" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D149" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E149" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F149" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G149" s="27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="4"/>
+      <c r="C150" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D150" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E150" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F150" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G150" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D152" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="E152" s="32"/>
+      <c r="F152" s="32"/>
+      <c r="G152" s="33"/>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="12"/>
+    </row>
+    <row r="154" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B154" s="2"/>
+      <c r="C154" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G154" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B155" s="2"/>
+      <c r="C155" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D155" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E155" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F155" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G155" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="4"/>
+      <c r="C156" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D156" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="E156" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F156" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G156" s="36"/>
+    </row>
+    <row r="157" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="158" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D158" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="E158" s="32"/>
+      <c r="F158" s="32"/>
+      <c r="G158" s="33"/>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B159" s="2"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="12"/>
+    </row>
+    <row r="160" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B160" s="2"/>
+      <c r="C160" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G160" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B161" s="2"/>
+      <c r="C161" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D161" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E161" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F161" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G161" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B162" s="4"/>
+      <c r="C162" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D162" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="E162" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F162" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G162" s="36"/>
+    </row>
+    <row r="163" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="164" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D164" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E164" s="32"/>
+      <c r="F164" s="32"/>
+      <c r="G164" s="33"/>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B165" s="2"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="17"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
+      <c r="G165" s="12"/>
+    </row>
+    <row r="166" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B166" s="2"/>
+      <c r="C166" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G166" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B167" s="2"/>
+      <c r="C167" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D167" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E167" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F167" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G167" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="4"/>
+      <c r="C168" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D168" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="E168" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F168" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G168" s="36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D170" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="E170" s="32"/>
+      <c r="F170" s="32"/>
+      <c r="G170" s="33"/>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B171" s="2"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
+      <c r="G171" s="12"/>
+    </row>
+    <row r="172" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B172" s="2"/>
+      <c r="C172" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G172" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B173" s="2"/>
+      <c r="C173" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D173" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E173" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F173" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G173" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B174" s="2"/>
+      <c r="C174" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D174" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E174" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F174" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G174" s="27"/>
+    </row>
+    <row r="175" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="4"/>
+      <c r="C175" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D175" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E175" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F175" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G175" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="19">
+    <mergeCell ref="D170:G170"/>
+    <mergeCell ref="D139:G139"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="D152:G152"/>
+    <mergeCell ref="D158:G158"/>
+    <mergeCell ref="D164:G164"/>
+    <mergeCell ref="D79:G79"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D115:G115"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="D131:G131"/>
     <mergeCell ref="D33:G33"/>
     <mergeCell ref="D39:G39"/>
-    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D52:G52"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="D15:E15"/>

</xml_diff>